<commit_message>
Get daily reddit data: Tue Apr 16 08:08:22 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_21.xlsx
+++ b/data/2024_04_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C423"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2080 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1c5a4q1</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tipping question </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5a4q1/tipping_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1c597co</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Nude Pink Acrylic&amp;Aqua Pink Top Coat</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c597co</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1c588v2</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>My Spring Fairy Nails</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgn045pk1suc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1c55b9s</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Can someone tell me why my ring finger is never the same shape as my other fingers? Do I just suck at shaping?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c55b9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1c53qom</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>I would love to hear your thoughts on this advice for weak, brittle, bitten nails.</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h8u1goavquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1c52gq8</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>which nail shape would suit my hand best</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6i7tyihokquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1c51pii</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Why do my nails turn clear?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2jhts9tequc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1c50fpc</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>My natural BIAB gel art VS inspo pic of press-ons on by Enroutenails on etsy.com/uk</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c50fpc/my_natural_biab_gel_art_vs_inspo_pic_of_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1c4zypj</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>What are your best do’s and dont’s for long nails?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4zypj/what_are_your_best_dos_and_donts_for_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1c571r2</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink pink </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uovxwyh0pruc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1c56zfj</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Starting to do my own nails😬</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5i9fpdfcoruc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1c56xzj</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Gel-x file question</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c56xzj/gelx_file_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1c55aps</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Love a fresh mani 💅🏻</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nponhzs8ruc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1c5510u</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>If I have a nick on the side of my nail, could builder gel save it?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5510u/if_i_have_a_nick_on_the_side_of_my_nail_could/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1c52ybr</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Just wanting to show off the new nails:)</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hc2nrpnoquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1c52e3u</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Not so great.  But husband's choice</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n70comv2kquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1c51kb7</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Brand new to doing my own nail art, pretty happy with how this turned out</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6v3ve2jpdquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1c50lp8</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thought? Improvements? </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a3o9ddha6quc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1c50itp</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Thoughts on nail shape?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t4jy33o5quc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1c50ayo</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>What do you think of these press ons?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c50ayo</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1c501n3</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Natural nails 🥰🍃</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c501n3</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1c4zrfj</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Love vibes 💗💞</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgdwmqrvzpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1c4zned</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>UV nail box?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4zned/uv_nail_box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1c4zk5s</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed 😍 </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1zc1rtdypuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1c4z71c</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Please don't be mean, but why do my nails look so bad?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4z71c</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1c4z4lq</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nails would go with this for prom ~ preferably long-xl length </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aiwb7eo5vpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1c4z347</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>The cat eye is cat eyeing😝</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwmc2c4uupuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1c4yv9u</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>LA Girl - Flaunt</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4yv9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1c4ys7a</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Loving it!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xddrzzopspuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1c4y33s</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>She’s pink she’s white</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n3392gunpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1c4xg4n</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Ladybug Nails 🐞</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4xg4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1c4x4ii</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>90s Spring Easter Summer Popsicle served</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4x4ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1c4wwqs</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Can i overcure basecoat?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4wwqs/can_i_overcure_basecoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1c4wh5z</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>First time trying square and I love them</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4wh5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1c4w6cu</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Can i mix nail primers?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4w6cu/can_i_mix_nail_primers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1c4vvbu</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Hoping this one will remain up 🥺🥺</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wn121zdb8puc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1c4vybj</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Cute and classy</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/doplqklu8puc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1c4vhg7</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Envy Strengthener Original </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4vhg7/nail_envy_strengthener_original/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1c4tdk9</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I've only ever used regular nail polish...looking for suggestions/advice on long-lasting manicure options!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4tdk9/ive_only_ever_used_regular_nail_polishlooking_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1c4uoqx</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Springtime gnome set</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4uoqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1c4o549</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail art brushes cleaning </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4o549/nail_art_brushes_cleaning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1c4l328</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Bridgerton inspired nails(I don’t know what character as I haven’t watched it yet)</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4l328</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1c4jol8</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>My nail journey so far</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4jol8</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1c4tq1s</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Too bubblegum pink for my skin tone? Panic-pivoted halfway through the “neutral pink translucent” mani on my natural nails thinking it looked awkward…</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4tq1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1c4t2d1</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Had them for a week</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4t2d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1c4t16w</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I just love this white-silver magnetic gel polish from Mayor's Silhouette set 🤍</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4t16w</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1c4szop</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Cherry blossom nails 🌸</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvxh5x65oouc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1c4spft</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Added a little chrome to my French acrylics</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4spft</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1c4sn1l</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Trying to rock short nails with polgel. I was brave and did my toes as well. Haven't tried doing my toes in many years.</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4sn1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1c4sck7</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Went to a new salon. Got an uneven French and now after cleaning the house the top coat is coming off. Never happened before</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4sck7</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1c4s906</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Press on help</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4s906/press_on_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1c4qnv6</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Guide me</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4qnv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1c4q087</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>my tech is nail-chelangelo and i am her masterpiece</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4q087</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1c4phfx</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Nail tech refusing to do my nails because of sweat on my hands</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4phfx/nail_tech_refusing_to_do_my_nails_because_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1c4p9cf</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>🔮</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ewe8z7jxnuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1c4ntos</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>New pink nails 🍓🥛</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00wjnd1ymnuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1c4md2m</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>🌼 Ombre pink to white + flowers!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8ofh9jqbnuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1c4lvmg</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Silver is my favorite color</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2em8pwq7nuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1c4k0d9</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>This look nice I guess?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4k0d9</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1c4jvyt</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring blue. </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb627mjrpmuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1c4jhdc</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Are the jewels too much?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/bountifulstupendousbufeo</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1c4io9h</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>How is it?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsv6so6kcmuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1c4ijk1</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Feeling funky 🕺🏽</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4ijk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1c4iaxz</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Nail Growth Plan.. I’d like the experts to weigh in.</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c4iaxz/nail_growth_plan_id_like_the_experts_to_weigh_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1c55kxp</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Australia specific - drugstore base coats/basics? Getting back into nails after a long break.</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bea6ahlcbruc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1c56egt</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>First time trying Death Valley Nails and I am obsessed now thanks 🫣</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c56egt</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1c5685w</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Dupe for Olive and June in shade LD?</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c5685w/dupe_for_olive_and_june_in_shade_ld/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1c55plu</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Nail game getting stronger</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54nxdasgcruc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1c54a53</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Can anyone help me identify this polish? It works GREAT and doesn't yellow my nails and dries almost instantly</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c54a53</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1c53yj9</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>china glaze top coat</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c53yj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1c52vqb</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>I have never worn a polish so vibrant 💙</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36ajsg53oquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1c52uwh</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>I always forget how luxurious a simple creme can feel</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hfemzlwnquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1c51vxs</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>How do you stay positive after cutting your nails short due to a low break? (Before/After)</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c51vxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1c51ko5</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>mother moon approaches. 🌘🌑💫✨</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c51ko5</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1c50v1l</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Ethereal Pigeon (Feb 2024 PPU) 🐦✨</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c50v1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1c50ugk</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Zipper stencils experiment</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c50ugk</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1c50pt7</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Glam Polish - Almost a Princess</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mny1iy77quc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1c50ozi</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Kites</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c50ozi</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1c501ku</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Had a crappy day but my nails has turned them around</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c501ku</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1c4zxgs</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Fruity nails 🍍🍓🍌🍉</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4zxgs</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1c4zehl</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Having fun going through my ILNP order! Here is Highline with its green and bronze shift:</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4zehl</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1c4x0jy</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Nail break</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkm68ld8gpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1c4y2st</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>My nails feel like springtime</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4y2st</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1c4xsaf</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Glitter nails 💜 glitter thread</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4xsaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1c4wnon</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginning my nail growing journey and matching my plants 🌱 </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d673omdodpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1c4wm9a</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>I’ve been wearing Sand Viper from Mooncat the past few days and it reminded me of something but I couldn’t put my finger on it. I realized while making lunch today that it’s the color of bologna 💀</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7v0psqfdpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1c4w1s7</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Siren's Deceit ✨️</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4w1s7</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1c4v9wp</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Polished for Days - Raspberry Chocolate</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4v9wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1c4utb8</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>looking for help!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c4utb8/looking_for_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1c4rv2o</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Proximal nail fold rehab</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc8zc7wbgouc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1c4u0vv</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Truth or Dare ! Monarch Lacquer</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4u0vv</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1c4tse6</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>2 weeks later, Cirque Colors. MADDER</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4tse6</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1c4tjhn</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Chrome always chipping?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c4tjhn/chrome_always_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1c4s99h</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Hidden suprise blue glitter</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c4s99h/hidden_suprise_blue_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1c4s7cl</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>When the color is so pretty in the bottle but awful on your hands</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4s7cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1c4rzr2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Looking for GELCARE Hourglass dupe in regular polish</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvfkfcq9houc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1c4qckl</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>4/20 nails a little early</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4qckl</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1c4ppzj</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Help with chipping?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c4ppzj/help_with_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1c4osuz</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Nude Floral Mani in April!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c57ddgertnuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1c4id23</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>First post! And first time I feel like I painted my nails almost perfectly!</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyp88w5y8muc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1c4nwvw</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>First thermal 😍</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wk0cxwdmnnuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1c4nh85</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Recovered nail biter</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4nh85</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1c4mzzv</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Rainbows &amp; Chaos - wearing the entire BKL Six Crimson Cranes collection at once</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4mzzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1c4m2v3</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Help me find the perfect color to match my bridal bouquet!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqiu8d9g9nuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1c4kgpu</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Pi Colors - Night Terrors</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4kgpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1c4j6b2</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you do with runny nail polish? </t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c4j6b2/what_do_you_do_with_runny_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1c4ifjg</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c4ifjg/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1c56k7g</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>This weeks fill</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c56k7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1c56c4a</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c56c4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1c554qe</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Blue and white china "Delft Blue" nails!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c554qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1c54mxj</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Progress!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c54mxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1c5301s</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Witchy spring set</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5301s</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1c525q1</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>A nail set I did today!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwwiijn8iquc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1c50x1p</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Notebook nails 📓 💅 📝</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c50x1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1c4yxna</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>I tried to give myself a marble effect, what do you think?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxok9jgttpuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1c4unhw</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Springtime gnome set</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4unhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1c4ty4v</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Gemstone nail attempt with gel</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4ty4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1c4ta1l</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>I’m in love with this my work 🥹💔</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4ta1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1c4r61s</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Spring mani on my aunt🌸</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff2qjwn9bouc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1c4nkan</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Hello Kitty set 🐱</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4nkan</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1c4k2bu</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Client request</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c4k2bu</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1c4hmly</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Dreamville inspired nails</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhhexhlyzluc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr 17 08:08:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_21.xlsx
+++ b/data/2024_04_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C423"/>
+  <dimension ref="A1:C588"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7624,6 +7624,2811 @@
         </is>
       </c>
     </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1c63hh7</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Tried something new</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kpg9tghjozuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1c62vxr</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Is the nail filing machine thing worth investing for doing your nails at home?</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c62vxr/is_the_nail_filing_machine_thing_worth_investing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1c62ogr</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Trying to work out which shape to make my nails. I cant have them painted but like to keep them nice, what shape do you think would work?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxix0ud5fzuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1c62gul</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>First post! Reminiscing summer 🍋</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fp5md20qczuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1c62559</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Butterfly bday nails 🩷</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6emi6br19zuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1c623j4</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>First time doing nail wraps on myself. How did I do?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv6nkd9k8zuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1c6200a</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>some of my last sets!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6200a</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1c61zh7</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>first time using hard gel :)</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c61zh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1c5zxd1</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Tile nail art!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5zxd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1c5zcax</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Second time trying forms + first time doing 3D Art</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5zcax</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1c5uvup</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>My favourite nail polish</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7ew376hfxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1c5r3rx</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Vaguely Kingdom Hearts Inspired Mani-Pedi</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5r3rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1c5pgxs</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>This precious hand-painted design my nail tech was able to replicate today…</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5pgxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1c5ovlf</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>How often should I get a new set of liquid gel nails?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5ovlf/how_often_should_i_get_a_new_set_of_liquid_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1c5nqsj</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to Acrylics </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5nqsj/new_to_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1c5lged</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>What do I do about this ? I had a small break :/ just wait for it to grow out? (Ring finger sidewall)</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt6f349zivuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1c5msh4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Help with growing out nails</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5msh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1c60u2v</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>new set, loving the ombrés lately</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwz2nujnvyuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1c5i28a</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>How do I fix these press ons to make them look more natural?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5i28a</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1c5fi5v</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Nail lifting</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5fi5v/nail_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1c5dlhj</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I need inspo and pintrest aint hittin</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5dlhj/i_need_inspo_and_pintrest_aint_hittin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1c60rg0</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Help getting my nails done for prom tomorrow what shape would look good on me</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu0fpenvuyuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1c6081c</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>my favorite nail art i’ve done on myself</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6081c</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1c5zxul</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Unpopular opinion</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5zxul/unpopular_opinion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1c5zwpq</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>One color is never enough 😅</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc0o7evlmyuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1c5zb2e</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>💅🏻</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhbnwm5zgyuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1c5yxwd</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Fresh pink set 🩷✨</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld32ed1rdyuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1c5ylnk</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Y’all liked my last set so much, here’s my current one.</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5ylnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1c5y5g5</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Painting Cherri Bomb from Hazbin Hotel✨🐍</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5y5g5</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1c5xzsp</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>First attempt at cat eye nails</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5xzsp</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1c5xrhv</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>I should organize these 💅</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7uxh9in3yuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1c5xphc</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Sunset nails - ESSIE MULTI FACETED</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7us5dek63yuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1c5xhiq</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>colorful pastel french tips (done by my manicurist)</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5xhiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1c5xc1k</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Do you prefer long or short?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5xc1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1c5wt1g</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>still practicing frenchies but what do we think?</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5wt1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1c5wshj</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>For our family friend who's running in the London marathon this week</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5wshj</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1c5wgcx</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>help! damaged nails</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ooftg6jasxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1c5wdy8</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>nude-ish with sparkles on natural nails (was a nailbiter all my life and recently was able to stop)</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4se5oeiprxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1c5ver7</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>builder gel + chrome (my real nails!) 🦄🐚🪩</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6c2m7h8pjxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1c5v5kb</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Flirty nails</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5h6t8mdnhxuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1c5uq66</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Why does this happen?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tg1o529exuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1c5umeq</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Pastel chrome 💜💙</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5umeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1c5u9mm</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Haven’t posted here in a while, here are my latest babies</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5u9mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1c5u61j</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic nail starter kit recs ? </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5u61j/acrylic_nail_starter_kit_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1c5u5m4</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>How to get long, strong nails that don’t chip or break?</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id0hwcdt9xuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1c5t8a2</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Wild basin gotta sponsor me for how good this looks!</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5t8a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1c5t6mf</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>i’m just a girl</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5t6mf</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1c5t3er</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Flower nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4s4gnrt1xuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1c5skci</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>I love how this effect looks on my nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61zngp21ywuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1c5sdxx</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Leopard Print (black and white)</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5prewbqwwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1c5s9jo</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>To all my short mail girlies. I love you😘</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dagfw2otvwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1c5rwn8</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Dear friends! I have a new fave! 😍 Look at the little dots!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5rwn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1c5rp9h</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>I'm in love with green💚</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d28qtobrrwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1c5rhor</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Press-On Set By Me 💗</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2x0za97qwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1c5rgfw</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>I have recently started growing my fingernails after years of picking and biting them. I have noticed as they are growing longer they are going a pink colour. What does this mean?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5rgfw/i_have_recently_started_growing_my_fingernails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1c5ra0y</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>There is just something about fresh pinks</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcmqfeimowuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1c5qj6c</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Press on Set By me 😚</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rgmd8k9jwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1c59tnm</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>guys help! why do my press-ons look so fake 😭😭</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c59tnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1c5pslq</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>🤍 Painted Polish Boos Cruise 🩵 Another Halloween shade that is perfect for Spring! 🌸 I haven't had a white polish in a long time. This formula is absolute perfection!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5pslq</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1c5ozye</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>How much?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5ozye/how_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1c5obyv</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Stilleto or square?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nxe6mke3wuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1c5nxid</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>First time getting cat eye polish!!!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlw49i9i0wuc1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1c5ntzs</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>need some help</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujta4sbtzvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1c5ms43</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Cherry cola nails 🍒🥤(they don’t sell cherry cola in my country, so this has to do)</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5ms43</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1c5mpgh</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Topcoat chips when neon pigment powders are applied to inhibition layer of gel color.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5mpgh/topcoat_chips_when_neon_pigment_powders_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1c5mkid</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Spruce &amp; Sarah</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5mkid</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1c5mjb3</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Do you like that tone, would you like it?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dglj5eaiqvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1c5mita</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Why the lines?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykv4klbjqvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1c5m6py</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>DIY Jade/Emerald 💅 took “only” 3 hours of my life</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5m6py</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1c5m62d</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Any advice of how to take care of my natural nails?(they're so fragile)</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ek6exc10ovuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1c5m082</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>tips for keeping nails healthy as a barista?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5m082/tips_for_keeping_nails_healthy_as_a_barista/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1c5ll7g</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Pinky girly nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyq5oxaxjvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1c5lj6p</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Self taught and practicing</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5lj6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1c5l5ic</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Did them by myself! How did I do?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xn3uzlugvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1c5kvwj</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Golden yellow stripy summer vibes ✌🏼 BIAB! </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnstoygwevuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1c5kppe</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>First time I've made them super long</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5kppe</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1c5korn</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Xenomorph alien nails 🛸🪐🖤 self taught</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5korn</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1c5kbr7</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>I don't know why they look beige, but they're pink and rhinestone</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5kbr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1c5k9j2</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Does this color suit my skin tone?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5k9j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1c5jym4</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went to the salon for the first time </t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhm8lgf78vuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1c5jtxd</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>just a cute simple flower design :-)</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5jtxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1c5jiir</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Did them by myself, how does it look?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy83cdn25vuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1c5jbec</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>My new go-to, when I can't pick between neutral colors and uplifting glitter:</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5jbec</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1c5iygp</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Base coat on top coat?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5iygp/base_coat_on_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1c5ixed</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>🤍🧿</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sqza40dv0vuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1c5hc7q</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Created my first set of press ons🍓</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5hc7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1c5hbyd</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Nail Ideas?</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c5hbyd/nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1c5hbjk</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Newbie</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5hbjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1c5h0gh</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Black or white ? ⭐🌙</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5h0gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1c5gykp</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Pink and purple shorties</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tz6jqj06muuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1c5gudh</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>First timer</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ogebtbcluuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1c5gpc7</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">chome effect </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67z0lyb9kuuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1c5gl9y</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got something out of my comfort zone this time </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccibnfmdjuuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1c5fhfn</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>These cost $90 in my city 🇨🇦, how much is a full set of long nails in yours?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8cm2gwbauuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1c5eebw</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Help finding color</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5eebw</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1c5d5ie</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Are they any better? 🥺</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5d5ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1c5cdxg</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Blue holo is life 💙</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkwer04eftuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1c63g4u</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail mail skittle! </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/szrorua2ozuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1c62ejd</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love the length and the color </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfxik0x0czuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1c61neu</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I'm sticking with the navy! 😉</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/lyYMBSB</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1c60mfp</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>PFD Lush</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c60mfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1c60l1q</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to avoid bubbling </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c60l1q/how_to_avoid_bubbling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1c60brn</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Green Goddess Naked</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kxf7qdsmqyuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1c5zgke</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Orly "The Floor Is Lava"</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6979p5diyuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1c5ypj8</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Starrily Amulet</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5ypj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1c5ydba</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Sassy Sauce — Shaken not stirred</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5ydba</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1c5y5ux</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Blossom</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5y5ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1c5y1ky</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Nude thermal polish recs?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c5y1ky/nude_thermal_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1c5uoqn</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>cirque jellies really take the cake</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7m9ytnxdxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1c5tnl3</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Hema Free Allergy</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c5tnl3/hema_free_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1c5saxt</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>help me find this polish!!!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6ijz0e4wwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1c5x5ho</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Zoya 50% sale &amp; polish recycling</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5x5ho</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1c5wgn4</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Pheonix Chibi Chibi</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5wgn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1c5w4p7</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Mediterranean Tiles!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5w4p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1c5un61</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>I’ve got a neon addiction 😅</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhtoii0ldxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1c5u84c</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>How to get long, strong nails that don’t chip or break?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hg35s4daxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1c5tlpm</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Dupe Help: "Made in Jade" by Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5tlpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1c5tj84</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Polish and Pokémon</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5tj84</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1c5tcbo</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Why does this happen?</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19yva6lm3xuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1c5sbx2</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Amazing Polish and Potentially Unpopular Sassy Sauce Opinion</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5sbx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1c5s9tj</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>I'm really not.</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5s9tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1c5roh8</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>👻 Ghosts of Hecate 👻</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5roh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1c5rmdf</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Will cuticle oil still work with clear polish on?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c5rmdf/will_cuticle_oil_still_work_with_clear_polish_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1c5r9wl</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Gotta love the glow 😍</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5r9wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1c5qjcd</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Mooncat Aphrodisiac, Moonrise and Portrait of an Introvert … a true INFJ-A / INFJ-T manicure</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kequ7uajwuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1c5q0y9</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I almost got too lazy for magnetics, but Cadillacquer’s chaotic colors pulled me right back in 💕</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/epvmqvdlfwuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1c5pwip</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>🤍 Painted Polish Boos Cruise 🩵 Another Halloween shade that is perfect for Spring! 🌸 I haven't had a white polish in a long time. This formula is absolute perfection!</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5pwip</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1c5phz9</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>This polish won’t photograph!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5phz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1c5o01u</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Dry, peeling nails after regularly polishing. What to do?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bi6t6br11wuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1c5nq8z</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Papillon shimmer</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c5nq8z/papillon_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1c5nkco</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Loving these blues lately</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewbagaltxvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1c5ndsm</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Starrily "Peach Glow"</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma1605siwvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1c5mowj</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Sparkly Yellow Nails for Spring (ILNP)</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5ki0hcrrvuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1c5mhvt</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Phoenix - Boolba PPU Jan/24</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5mhvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1c5m5mr</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>larkspur</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5m5mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1c5m4m9</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Magical magnetic (cirque colors Cassiopeia)</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5m4m9</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1c5m3dz</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Bkl the twin adlers</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5m3dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1c5lu3x</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Holos are so pretty ✨🌈</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5lu3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1c5lej1</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Showstopper ✨</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5lej1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1c5lctz</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Added some dragon</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5lctz</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1c5l2w1</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Cirque what is you doing???? [Updates to Cirque's Loyalty program]</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zt3mcc7zfvuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1c5kp20</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Stagnant Water</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5kp20</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1c5khub</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Probably my favorite set I've gotten</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5khub</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1c5k75j</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Dazzle dry vs green flash</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5k75j</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1c5k1co</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>It’s only Tuesday, but so far this manicure has been the best part of my week.</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5k1co</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1c5jj8h</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>I still can’t get over how holo this polish is!!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ja7vyq75vuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1c5j1vd</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Why isn't there more hype around Picture Polish Curable?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ayh089r1vuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1c5iwi4</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>🏅❤️Fave Reds❤️🏅</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5iwi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1c5hdcx</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Misery is My Favorite Color 💙🖤</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5hdcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1c5hbdo</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Essie gel couture color for engagement?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c5hbdo/essie_gel_couture_color_for_engagement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1c5h15c</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mannequin-ish nails </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/054tpfrpmuuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1c5ghrf</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>My last two untrieds!</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5ghrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1c5g1id</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Dupe request please</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3129p4yeuuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1c5ab0r</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Need nail shape advice</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5ab0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1c5cek8</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Blue holo 💙</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiro1ivlftuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1c5xv02</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Painting Cherri Bomb from Hazbin Hotel💕</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5xv02</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1c5xivr</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Hot Girl Spring</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr3hnncj1yuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1c5wzs0</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Today’s nails for my client. I love the color combination 😍</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zje7zjyvwxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1c5wxo1</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Bling Bows and Polka Dots</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r94sx15ewxuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1c5wkdo</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Took way longer then I’d like to admit</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5wkdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1c5mhb7</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>DIY Jade/Emerald 💅 took “only” 3 hours of my life</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5mhb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1c5l23f</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>amiga cheetah ⭐️💕</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5l23f</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1c5jswz</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>What do you think about my new work? 💛</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5jswz</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1c5hhw6</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Citrus nails! 🍋 🍊</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4pctowaquuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1c5edo5</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Pinterest inspo</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5edo5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr 18 08:09:12 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_21.xlsx
+++ b/data/2024_04_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C588"/>
+  <dimension ref="A1:C703"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10429,6 +10429,1961 @@
         </is>
       </c>
     </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1c6xeyz</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>My nails keep.. peeling?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8r7hjk7x6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1c6x812</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>what is best for soft gels? (gel x)</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6x812/what_is_best_for_soft_gels_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1c6wysl</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first proper client! How did I do? </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxy36xo0s6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1c6wvie</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Purple and black are a perfect match.</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1yolc8qq6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1c6vytl</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>What nail color would compliment my olive skin tone?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlogml8dg6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1c6vuj4</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Wine red, do you like it?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxsgfiwve6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1c6vmx5</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Paid $65 for my daughters nails for prom.</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6vmx5/paid_65_for_my_daughters_nails_for_prom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1c6ve5e</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Bling n long 😍 bday nails for aries szn</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y0dtab3a6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1c6vczl</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>It took 3 hours but it was so worth it!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6vczl</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1c6uskw</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ni2goolo36vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1c6upvx</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>My HelluvaBoss nails</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdf7tz0v26vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1c6uitw</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>love my nail tech</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwwulfwr06vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1c6ugau</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>New to nails!</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6ugau</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1c6uasy</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Can I just apply polygel to just half my nail to help build length?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6uasy/can_i_just_apply_polygel_to_just_half_my_nail_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1c6took</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>How to keep a full set on longer</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6took/how_to_keep_a_full_set_on_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1c6te1r</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Here's a better photo of my nails! Pink gel, unicorn chrome. With clouds &amp; stars☁️🌟</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf2yvr1fp5vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1c6puup</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Thickness of soft gel vs acrylic vs press ons?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6puup/thickness_of_soft_gel_vs_acrylic_vs_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1c6oupc</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Nails Keep Splitting</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l9uagrfl4vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1c6rdde</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Are cheap electric nail files okay to use?</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68akvsdy65vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1c6r6lq</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Did my sisters nails</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmicaoq755vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1c6r3kk</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7in974pi45vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1c6povh</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>SNS cracking?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuhwgr2es4vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1c6pnsg</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Best places to buy nail supplies?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6pnsg/best_places_to_buy_nail_supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1c6pb27</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Longest my nails have been in a minute, natural nails with dip powder. Been slacking with using my nail oil so cuticles are looking a bit rough.</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6pb27</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1c6oufe</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Anniversary nails (done by me)</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6oufe</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1c6n1bf</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Learning to do my nails at home</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km8d74zf74vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1c6kjdi</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Bit my nails my whole life and stopped recently (26 M)</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6kjdi/bit_my_nails_my_whole_life_and_stopped_recently/</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1c6idx8</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>HELP! SNS Dip Powder</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6idx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1c6hon0</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Can anyone recommend any sheer pink nail polishes that look similar to this? (Photo by Instagram nail artist “constantlypolished” used as an example)</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8pcq6ht43vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1c6lc6p</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie lollipop </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6lc6p/essie_lollipop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1c6krca</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>pink drink nails 🍓</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6krca</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1c6jasl</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Biab nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6jasl/biab_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1c6j5uy</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Okay these are now my fav spring set lol</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4y6zv1if3vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1c6iyvl</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Gold and Pearls</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6iyvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1c6itij</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple on my mind. 💜💟 I had been growing my nails for couple of months but they kept getting chipped. So I have cut them short again. </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk9azwkzc3vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1c6icfr</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love nail day 💕 </t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kw4suhj93vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1c6i451</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Rainbow skies</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/verdbzpv73vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1c67hpd</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Why do my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c67hpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1c6hewz</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Pink nails, unicorn chrome with clouds &amp; stars! My favorite set by far☁️🌟💅</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9gmdl9t23vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1c62bk1</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Best fill-in I ever got</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xubv9we2bzuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1c6h7fo</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Spring has sprung 🌸🌼</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6h7fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1c6gxeh</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Fallout Nails</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gd7k3chcz2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1c6gm49</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>What shape and length nails would look best on my hands?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6gm49</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1c6evec</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newest set! </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqrninkpk2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1c6e4s1</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Disco Ball Pink 🪩</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6e4s1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1c6doel</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Start your engines 🏁</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ljana1ac2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1c6djsk</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Looking for Peridot by Revel Nail</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lygc79bhb2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1c6deet</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Gel mani?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvvvfkcea2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1c6dcak</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">starter builder/hard/soft gel products? </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6dcak/starter_builderhardsoft_gel_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1c6dc6i</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>first time in a while i’ve been proud of my nail art</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6dc6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1c6daxz</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Keeping gel x nails glued on hands when you made them on a nail stand?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjrw3ito92vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1c6cf0y</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6cf0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1c6bzh9</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>One of my fav sets 🥹(Not my work)</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6bzh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1c6bqcd</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Too much ? Or just alright? (Set done by myself). Also an opinion on the gem in the center plz. Should I switch it with another color is it alright?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3i97dh9y1vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1c6a5k5</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>First time using cat eye polish</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6a5k5</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1c6a4rf</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do tlmy nails look okay or do they look too thick and chunky?? </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aa2uzlecm1vc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1c69zfg</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Cinnamoroll core 🌀</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ku9tsma9l1vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1c673pa</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b46hcyuv0vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1c66bvw</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Dual form with acrylic gel or gel x?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c66bvw/dual_form_with_acrylic_gel_or_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1c66a39</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Do you prefer French?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8v5j88bwm0vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1c65o33</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>My first time getting my nails done :)</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c65o33</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1c65ikx</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>First go at a full set gradient.</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eti6erttd0vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1c65198</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Spring Blue 💙</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c65198</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1c6wzqc</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Orly ColorPass Summer 2024</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o2bvpz8s6vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1c6rjb8</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>I love with this blue 💙</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6rjb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1c6qihl</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Linear Holo Taco Skittle</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6qihl</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1c6pl21</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Cloudy Dusky nail art</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyj72n8ir4vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1c6omrt</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>DIY Nail Stand</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tg9yt6nnj4vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1c6n7lv</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Slimey Glow 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g47ditbq84vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1c6mwx0</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>My reds 💖</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a937jcuo34vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1c6m7lq</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>soon needed some sparkle but it gives Christmas vibes 😅</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkkywdvc14vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1c6lxuh</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Polishes like Lament from Emily de Molly?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/me9vq00dz3vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1c6lboy</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Ether Dragon - Ethereal Lacquer 🐉</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6lboy</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1c6l8un</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>🍓 Pink Fruit Smoothie Nails</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6l8un</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1c6l2a5</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Do we like this on me?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6l2a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1c6krpe</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>[ISO] Mooncat</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c6krpe/iso_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1c6knv3</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Robin's egg, but make it ✨ sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6knv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1c6kcfo</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Changed my nails from round to almond, and rocking a space bandaid. </t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlt0ktisn3vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1c6k5cb</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>ISO metallic black</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6k5cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1c6jugn</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Come get me, summer. My nails are ready!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6jugn</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1c6jmsu</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>A Very Unmerry Birthday to us 🫖 🎂</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6jmsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1c6cbah</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>TTPD Nail!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rh5p0flj22vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1c6etme</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Does Emily de Molly have sales with any predictability?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c6etme/does_emily_de_molly_have_sales_with_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1c6gutg</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>I haven't done my nails in ages. Love them 💜</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6gutg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1c6ghwv</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>It’s giving glitter tennis ball</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88gyfhbcw2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1c6g7kd</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My sheer, short nails </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hbpekv9u2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1c6g3e2</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Sally Hansen</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6g3e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1c6fsgj</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>My first jelly sandwich</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6fsgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1c6fs3f</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Yoshi egg nails for my BF’s birthday 💚🤍</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofpuj2s6r2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1c6fpma</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>New polish got me feelin pretty 💃</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6fpma</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1c6fciq</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>best pink nude polish to help grow nails out?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6fciq</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1c6eaxw</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Went to a new nail salon yesterday... Safe to say I'm never going back</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c6eaxw/went_to_a_new_nail_salon_yesterday_safe_to_say_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1c6dgup</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Looking for Peridot from Revel Nail</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ts4hkjdwa2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1c6d2kf</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Recent nail combos</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6d2kf</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1c6a3od</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>trying a new shape… can’t decide if it suits me 🤔</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6a3od</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1c6963j</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>🏅🧡Favorite Oranges🧡🏅</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6963j</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1c6925j</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Might have found my new fave Spring color 💅🏽 OPI shade I Quit My Day Job 🌸</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9l9rtt3e1vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1c68krl</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Looking for the perfect pink OPI gel....</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c68krl/looking_for_the_perfect_pink_opi_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1c67zle</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Cirque - Elixir of Everlasting Life</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c67zle</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1c66j6s</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>She’s giving ✨ circus ✨</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c66j6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1c66hg7</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Who makes the best toppers?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c66hg7/who_makes_the_best_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1c66er9</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Hexcellent by Sassy Sauce changed my brain chemistry</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c66er9</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1c5zsca</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>dupe for PFD’s “catch ya later, dudes”?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c5zsca</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1c6vq0z</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fidget spinner nails! </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m5ov3njpd6vc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1c6u300</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Little hearts</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6u300</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1c6s7wi</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Look how cute this jellyfish is</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijs2lmlie5vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1c6o1yv</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>My first attempt at freehand character art, far from perfect but I think she's pretty cute 🧡</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/398bcet4f4vc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1c6kogx</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Pond-inspired nail art I did! Ignore the break on one, I did them Monday but forgot to take photos lol.</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6kogx</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1c6jn23</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goop 🌙 </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/028qdq6ti3vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1c6gjki</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>OK, so I I tried the flowers again I’m not great, but definitely better.</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tniecbznw2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1c6f7tk</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Hacker Nails!!! 💅</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6f7tk</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1c6dozw</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Start your engines🏁</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gp04fzydc2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1c6dg14</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>My freestyle chrome set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfh8ty2qa2vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1c6aihc</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Nanami Kento👔</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6aihc</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1c65kqh</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>First water marble :)</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gx64w8kke0vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr 19 08:08:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_21.xlsx
+++ b/data/2024_04_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C703"/>
+  <dimension ref="A1:C831"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12384,6 +12384,2182 @@
         </is>
       </c>
     </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1c7qsrr</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05yjqwy11evc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1c7q1yu</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Nail Tech Freezstyle</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f33df408sdvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1c7a67q</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Trendy bows</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7a67q</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1c7pjp9</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Clean girl nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2wiz5qemdvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1c7pgc9</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>rough wrinkly nail?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7pgc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1c7p6qw</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these, what do you think </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r67zwspbidvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1c7ozq6</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Glowy and cute🤍  Thoughts?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9b7sjo5gdvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1c7osy3</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Love my simple set ♥️</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omqzgcj2edvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1c7nz03</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Nude colored nails with heart detail and strass 💖 I love them!</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0dg96z85dvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1c7ndce</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Nails love</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qpqa6vezcvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1c7ncs5</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>What nail shape matches my fingers/hands?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7ncs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1c7n19r</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Ruined nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bif019c6wcvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1c7n0re</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>3D Fruit Nails</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7n0re</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1c7mv99</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>The one and only miss billionaire. Kitty Chan(set done by me)</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7mv99</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1c7m4l0</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Seeing long distance boyfriend, what nails to get?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7m4l0</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1c7m300</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>I use polishes a lot but my natural nails have become quite yellow which affects the look of my sheer nail polishes like Essie Mademoiselle; it looks so bad and not its usual pink at all. How can I fix my natural nails?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7m300/i_use_polishes_a_lot_but_my_natural_nails_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1c7llr6</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Silver chrome 🩶🤍</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9tq8sswicvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1c7ki8t</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>First magnetic nails</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7ki8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1c7k54c</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Tried the nail art for the first time</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7k54c</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1c7k049</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>First Timer, Give me some tips (Pun Intended)</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7k049</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1c7jfjs</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>The nails I did on my sister for my niece’s barnyard-themed birthday bash</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6x0z4dtzbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1c7iecx</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Nail help!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7iecx</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1c7i8le</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Are these too stark? I can’t tell if it looks bad at this point.</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7i8le</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1c7hyw0</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>original sylveon design!</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3ydq36vnbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1c7hx8u</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Went back to short and square 😊</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7hx8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1c7hvqq</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Cute lil spring nails I got 🥰</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ffdari6nbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1c7a0jf</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Recently started to get my nails done!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7a0jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1c7hh0u</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Blue is my fav colour 💅💎🌊</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4humlkxxjbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1c7h42x</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>First ever acrylics</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y66miaabhbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1c7gxm9</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Polish the tootsies</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7gxm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1c7gu5g</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Opinion: Glamnetic Press-On Nals</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7gu5g/opinion_glamnetic_presson_nals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1c7glca</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Trying chrome again! 💚</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyyxl12cdbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1c7ga5g</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>🍒🍒🍒🍒</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bx3fv7fzabvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1c7g7td</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Kerasal for finger nails</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7g7td/kerasal_for_finger_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1c7fmc6</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>They were supposed to be a silvery-blue. Instead they are just silver. I think I like them anyway. 🤷‍♀️</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9jug2p56bvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1c7fh81</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Finished painting winner/sinner Sir Pentious from Hazbin Hotel 🐍🥰 for his press on nail set ✨</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7fh81</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1c7fa5i</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Chrome Nails - Only Powder?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7fa5i/chrome_nails_only_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1c7ee3s</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mixed metal </t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0grwyegcxavc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1c7dixy</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press-On Recs for Classic Red Medium Almond  </t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7dixy/presson_recs_for_classic_red_medium_almond/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1c7dgqj</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Happy Spring!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00sopbfpqavc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1c7d9im</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>idk how to feel</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5lu9cd9pavc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1c7d0ip</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Horrible lifting </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7d0ip/horrible_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1c7chqu</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Baby boomer nails 💗</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6umkccg2kavc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1c7blid</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Is there any way to reshape the pink part of my nails?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzuxp7vkdavc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1c7bdgd</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Press Ons I Made for Bride</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7bdgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1c7aqd2</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>After weeks I finally painted them right</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7aqd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1c7ai2o</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Best Lamps For Gel Brands Without Their Own Lamp</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7ai2o/best_lamps_for_gel_brands_without_their_own_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1c7aepe</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>What would cause this?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7aepe</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1c7a5xv</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Java &amp; Romantique</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7a5xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1c7a5lr</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>My nail artist has stunned me yet again! Brights for spring/summer</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7a5lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1c79z09</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Desi nails</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c79z09</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1c79ywm</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjs4scy22avc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1c79l4l</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Hello spring 🦋</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c79l4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1c73eff</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Current Set and How-To Guide to My Process!</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vdtjcirp8vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1c779pb</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>A few of my favourite nails over the past year - Korean Soft Gel</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c779pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1c773rv</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>New nails feeling cute</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8vpavagh9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1c771y9</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>New little spring gems</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvyebm43h9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1c76wa0</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>got fresh nails for my cruise🚢</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nsi4ef10g9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1c76vxa</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Nail care + system help</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c76vxa/nail_care_system_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1c76oae</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the name of this ring that holds swatch sticks? I need to order more, but I don't know what to search for. </t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcl56zxee9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1c762q6</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Refill vs new set prices and tipping </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c762q6/refill_vs_new_set_prices_and_tipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1c73yty</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>birthday nails!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w6dj3k9u8vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1c73rxh</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Watermelon Jolly Rancher</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c73rxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1c73ouq</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Are videos allowed? Let’s see. My favorite set yet! Gel-X</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4maog6o2s8vc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1c73bt0</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>What to get instead of BIAB</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c73bt0/what_to_get_instead_of_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1c72jq5</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Damaged Skin/Cuts and Dry</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ghrm49cqi8vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1c6vs5v</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Green Tint?!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6vs5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1c6v8hm</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Beach inspired nails</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/445itg1e86vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1c731aw</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Uñas para una modelo (hechas por mi)</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hktuiazum8vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1c6zvdh</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>I did my own nails 🩷</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxqjqon7s7vc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1c6zgj9</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Pokemon! ♡</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hvrskffln7vc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1c6z7gv</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>spring bday nails!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2biogdudk7vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1c6xzgf</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>The worst feeling</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c6xzgf/the_worst_feeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1c7qdft</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Southern hemisphere autumn nails</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o9edix0wdvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1c7pkzs</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Yayoi Kusuma x Lacquer 22 Nails</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7pkzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1c7pbke</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Calcifer! </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c7pbke/calcifer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1c7njno</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Porcelain patterns</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7njno</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1c7mplf</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Dupe request</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mf49om22tcvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1c7l4s5</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe request for peach shimmer by iglow </t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjkvn98uecvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1c7in81</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>I know I’m very late but I absolutely love Lavender Sky jelly</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ofzbgkq9tbvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1c7h587</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>First holo. I don’t think I can use standard polish again ✨</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7h587</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1c7gyjv</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>This shade reminds me of childhood pool parties</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7gyjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1c7g2m5</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>I need this lip color as a nail polish! Any ideas?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sitlzh1g9bvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1c7ff18</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You Conjured Me Out of Hope </t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ey1skx2n4bvc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1c7fe68</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Midnight mistakes </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c7fe68/midnight_mistakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1c7djun</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>I recently got my first few Phoenix polishes. It was worth the month and a half wait.</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7djun</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1c7cegy</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Kerasal</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c7cegy/kerasal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1c70ekl</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>[nails] [help] need some help deciding what nails to get done</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/apj2xrq8y7vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1c7b4oh</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Updated the last mani I posted to fit my surroundings a bit more!</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7b4oh</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1c7a1dv</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Purples Compared</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7a1dv</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1c79523</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>2 polishes, 3 colors! Phoenix wins again.</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c79523</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1c790yp</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Springtime Purple 🪻</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c790yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1c78ots</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail stickers </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fdtpxhvs9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1c78hsb</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>River Spirit</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lo9t1bhr9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1c788hm</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Week old mani</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c788hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1c77ywv</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>I saw a RedditLaquerista wearing Shift in Perception by Emily De Molly so i bought Shift in perception by Emily De Molly</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/luc1onhln9vc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1c76wzl</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Maybe?</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33avgez4g9vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1c76rus</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Pahlish - Lolly</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c76rus</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1c76cey</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Well Hot Damn</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c76cey</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1c75wmt</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Rocking Kur Perfecting Nail Veil #4</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4ugrnht89vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1c75rsg</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Super Glossy Taco dupe?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c75rsg/super_glossy_taco_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1c74y5r</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Snow cone by Cirque Colors 💙💙</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c74y5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1c74tao</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Phoenix polish has my ❤️</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c74tao</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1c74ro6</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Polished for Days- Goblins are what dreams are made of?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1l2mfwrvz8vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1c735yy</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>This is your friendly reminder to moisturize</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c735yy/this_is_your_friendly_reminder_to_moisturize/</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1c73016</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>🏅💛FAVE Yellows💛🏅</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c73016</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1c72ohs</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>First step out of "normal" nail polish and into salon type nails?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c72ohs/first_step_out_of_normal_nail_polish_and_into/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1c72djf</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>An oldie but a goodie</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c72djf</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1c72c0l</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Lullaby 💤 🌙</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c72c0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1c6rkcf</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Staycation by ILNP</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6rkcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1c6pxhw</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>My first time working with rubber base gel &amp; doing a French tip, I’m obsessed with how it turned out!!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c6pxhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1c71hlu</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>The shift is unreal</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l6xrp3z498vc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1c70rhj</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Kale Nails 🌱</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c70rhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1c70p0t</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Desperately in search of a dupe! </t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/244uidg818vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1c6zxig</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Petition to normalize crackle polish again 😝</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvb3uo4xs7vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1c6y95v</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pokeball Nails! </t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t11kdsw087vc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1c7qjsb</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>How do I recreate this design? Please help🙏</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8p25tk2ydvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1c7o89q</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Black nails pierced w gems🖤</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqbo4s608dvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1c7mzfm</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>3D Fruit Nails</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7mzfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1c7m9ma</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Went for smoky and came out marbled</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyhrx3vuocvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1c7lrl6</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>My cat died on Tuesday.</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7lrl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1c7j86d</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>April showers bring may flowers (early?)</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnnahrp2ybvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1c7fgt2</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Finished painting winner/sinner Sir Pentious from Hazbin Hotel 🐍🥰 for his press on nail set ✨</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7fgt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1c7c2ta</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>I’ve missed my ✨ natural nails ✨</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7c2ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1c77vl5</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Showcase of the past year nail art</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c77vl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1c75fvs</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Kapping for myself what do you think?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jtt4mgkg59vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1c745eq</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Rate this free style</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c745eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1c70cei</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Sweet ribbon French 🎀</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scpctc3ex7vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr 20 08:07:01 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_21.xlsx
+++ b/data/2024_04_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C831"/>
+  <dimension ref="A1:C980"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14560,6 +14560,2539 @@
         </is>
       </c>
     </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1c8k7nw</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Pink handmade press on nails</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8k7nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1c8jkly</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>What is my fault when the gel does Not hold when doing Russian Gel Manicure?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wsdk0d21lvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1c8jh2q</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>(21M) About to trim my nails. Are they respectable for future reference? Rate-me</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8jh2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1c8iuo9</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail biting </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8iuo9/nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1c8hpzy</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>freestyle set</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8hpzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1c8ejt3</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Nail glue stickers love or hate?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8ejt3/nail_glue_stickers_love_or_hate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1c8ddzj</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>In the name of the moon, I’ll punish you!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8ddzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1c8bj8q</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>what’s the process for nail art this detailed? (cr ig:suzu nails)</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9qreckjvivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1c8b7dx</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Love this set 🌸</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7quyx9tqsivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1c8543i</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Do i want something that doesnt exist?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8543i/do_i_want_something_that_doesnt_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1c8gz2q</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>What causes peeling of the layers of gel? I think I wiped off the sticky layer bfor the french design.</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8gz2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1c8ggmk</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>So undecided on which style to pick today to do my nails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqlge0z04kvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1c8g2a6</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Not sure if I like them or not</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a137wej30kvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1c8g0fq</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Press-On Set By Me 💗</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q945zvskzjvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1c8fjru</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Yay or nay ?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8fjru</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1c8e9tb</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Weird nail ridges</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv84petdjjvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1c8db8h</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Tried some tie dye techniques, still working on perfecting…Happy 420🍃💨</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qibjgahjajvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1c8db5a</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Do these look like press ons?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8db5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1c8cyyk</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>My most random nails thus far</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdqkj1sk7jvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1c8cgkk</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Chrome White nails 🤍🩵💜 changes colours depending on light 🌈</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8cgkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1c8c4b9</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Gel X dupe with attempted mirror chrome silver french tip</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8c4b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1c8bl34</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>space nails</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hqepyoyvivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1c8b724</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Carmela Soprano called</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xb5yyljosivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1c8awqs</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfp92umbqivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1c8alp1</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Deep smile lines for my frenchies</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkqrbb7znivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1c8a1pb</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>💙 obsessed as always</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5946h7ljivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1c89qc7</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>This is the longest I've let them grow</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c89qc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1c898ul</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Morning sky 🌤️</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt7qznhidivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1c896j3</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c896j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1c893hm</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Proposal nails?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sdb4kh8ccivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1c88cuh</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>fresh set 🎀🐱💅🏽</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34sm7smx6ivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1c888xz</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>i’m 19 and newly licensed nail tech. i wanted some practice, and here’s the outcome!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c888xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1c86s6m</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>DND cherry pie dupe</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c86s6m/dnd_cherry_pie_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1c86pn0</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Floral blue set</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c86pn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1c86aiv</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>made my first press ons today!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fevxqhlrrhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1c85l74</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Daddy long hands</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6e6bilimhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1c85fcw</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Copper or creme?🎂🧡</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c85fcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1c850s6</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>A ring light makes all the difference!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c850s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1c84wt5</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Simple black, BIAB on natural nail claws 🖤</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11n04eiihhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1c84ke1</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>How to take off press on nails the same day</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c84ke1/how_to_take_off_press_on_nails_the_same_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1c83qmz</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>🩶</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4tie2cw8hvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1c83pe3</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>How long does a peel off base coat last?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c83pe3/how_long_does_a_peel_off_base_coat_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1c831cn</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Shifty ✨️</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c831cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1c82x19</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Broken nail fixes?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yk1n88703hvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1c80mr0</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Remove gel at home?</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbkpgiggmgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1c82blm</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>do we vibe with these? i’ve been doing my own nails for a while but haven’t ever really put too much effort into design. i think they look okay from a distance or a quick glance. ik i got gel polish all over the place :/</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c82blm</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1c820fk</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Hand sculpted Lisa Frank 3D Nail Art Charms🩵🌸🐬 so obsessed with how they came out!!!🩷</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c820fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1c81ddh</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>espresso themed! iykyk 🤎🤍</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c81ddh</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1c81c64</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c81c64/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1c816ec</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Handpainted nails from this and last week</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c816ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1c80yhk</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>I'm studying! please rate 0/10☺️</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yksd270sogvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1c80dy8</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Dashing Diva gloss strips</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c80dy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1c800cr</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>1 or 2 ?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c800cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1c7zuej</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am in love with my design </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr0fotypggvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1c7zorb</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Elle Woods-core on my last day of law school classes ever ⚖️💅</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef5cycamfgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1c7zn63</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1p9ul3afgvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1c7ze2o</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>What nail shape would be best?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1eq3ooddgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1c7ywvc</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Natural Nails - Spring Art</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7ywvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1c7vdn0</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>How do I fix this mess?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7vdn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1c7y8um</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Will sand ruin my acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7y8um/will_sand_ruin_my_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1c7qlba</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Any advice on how to recreate this look?? Inspo: ig @nailsbyaryna</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rqrnetkydvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1c7lpgj</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>cat eye gel + chrome 😍✨ • nail inspo by @rond_maki on Instagram</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hw1cfmtjcvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1c7xqvv</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do people get good pics of their nails? My photos don't do them justice. </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3u0jh0bx0gvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1c7xlp6</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Got new mani yesterday</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7xlp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1c7xcly</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish question </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7xcly/nail_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1c7x252</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>clean &amp; clear ✨</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7x252</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1c7wq97</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7wq97</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1c7vray</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can make my nails more dome like? </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7vray/how_can_make_my_nails_more_dome_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1c7ulem</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>A little French moment for a friends wedding</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrrs8cqp9fvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1c7u3n9</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>pearlescent</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7u3n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1c7toj7</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Hols Nails, how much does this cost?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7w4n7n30fvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1c7thpf</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>More sun more bright!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73b4r65xxevc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1c7suwq</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Like it 🤩</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eog7d3bqqevc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1c7rzn3</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Polka dots for Spring! 🫧</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3gcqmiyfevc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1c7rjsb</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you shower with acrylic nails? </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c7rjsb/can_you_shower_with_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1c8je0u</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Whats wrong few of my customers break her nails, but never mine at russian manicure?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38ymz0vxykvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1c8j22n</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>4/20 nails 🥬</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/chpbxya3vkvc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1c8ioez</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Mooncat Haunted Forest</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8ioez</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1c8hypy</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Per Se</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8hypy</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1c8g3li</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Are y'all tired of Cock a Doodle Doom pics yet?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9wvsmjqg0kvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1c8fwgo</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>I am of the firm opinion that ILNP's velvet collection has been slept on.</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bug9cl8fyjvc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1c8fsmg</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Mooncat Bubbles? 🫧😔</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8fsmg/mooncat_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1c8f8lo</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Came across this sponsored post for Hot Cheeto Cuticle Oil while searching nail health on the Google...</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21wqjc07sjvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1c8ert4</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Late Checkout 🔮👻🔮 by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcx4a750ojvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1c8eran</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Nails done for my “spring fling” party!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqaz0avunjvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1c8ek5s</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Flakie Holo Taco is way more packed than I thought! 🖤💿</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3djkrrz1mjvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1c8e9yn</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Alpine Snow + Funny Bunny?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8e9yn/alpine_snow_funny_bunny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1c8e8vv</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer “Archived” meaning?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8e8vv/bees_knees_lacquer_archived_meaning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1c8d4ce</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Am I Crazy?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8d4ce</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1c8cz60</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Black Magic with a sprinkle of Fairy Dust 🧚</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8cz60</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1c8coqu</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>trying to rock short nails 😭</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzk5v6325jvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1c8ciyc</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Swifties, what colours are we vibing with for TTPD?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8ciyc/swifties_what_colours_are_we_vibing_with_for_ttpd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1c8b6y0</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Retro Rainbow Skittle on this decidedly un-Spring day</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8b6y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1c8akqq</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dull Stress </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frgijfirnivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1c85j9b</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Cirque colors new releases in Harlow &amp; Co</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c85j9b/cirque_colors_new_releases_in_harlow_co/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1c88x7n</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Craziest thing you’ve done for nail polish.</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c88x7n/craziest_thing_youve_done_for_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1c88rh0</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>I want to know your STATS! How many polishes do you own? How long have you been collecting? How many do you want to declutter/sell? Etc!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gol0q18v9ivc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1c88eoi</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>ILNP plain jellies coming soon</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c88eoi/ilnp_plain_jellies_coming_soon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1c87knk</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Trying to decide on a peachy pink jelly for my sister’s bridal nails</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c87knk/trying_to_decide_on_a_peachy_pink_jelly_for_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1c874u1</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Mod about you</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u50s4x91yhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1c86zgj</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Pink is the colour</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c86zgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1c86ipe</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Season 🌸💖</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e70py4rfthvc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1c86exp</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>i always reach for this green when spring comes around 🍀🍀</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pod5515nshvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1c85x5o</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Glowiest polish I’ve worn to date. Parrot Polish “Kallani”</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c85x5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1c85iai</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y07c87kwlhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1c852ss</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Death Valley flower toppers 🪻🌱</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c852ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1c84js3</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>My nails keep breaking at this length</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z14q32vehvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1c83wn5</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Saw this gorgeous new one from Kathleen &amp; Co and some shots made it look like a red shimmer, but it's more of a pink. Does anyone know of a polish like this (taupe/brown base) with a more red shimmer? [pic not mine ofc, it's a promo shot]</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs9rsrhy1hvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1c83wej</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Nice day for Nice Day For a Cardigan 💜</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c83wej</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1c83tt3</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">UK gang where are we getting our horseshoe magnets from </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c83tt3/uk_gang_where_are_we_getting_our_horseshoe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1c83oh6</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Polished for Days - Look Alive</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c83oh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1c82tfr</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>ILNP Elsa</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c82tfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1c8249d</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>ILNP - Up Above (with Polished For Days soft focus base coat in Plum Taupe)</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqpl6mz1xgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1c821q7</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Absolutely love this shade!!</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgj6rrjkwgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1c81vyr</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>This spring skittle got me drooling 🤤🤤</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n23m2i9fvgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1c81qdn</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tell me your favorite vampy shades </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c81qdn/tell_me_your_favorite_vampy_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1c80chn</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Death Valley Nails promo featuring a magnet hack.</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j29yf0t8kgvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1c806va</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Bees Knees are really killing it at the moment imo</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c806va</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1c7ztj9</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Nail Photo Pro-Tip</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kaxwlhmjggvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1c7zna2</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Elle Woods-core on my last day of law school classes ever ⚖️💅</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tlvraytafgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1c7zeuv</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>People who find ILNP Overcoat flattering, what other neutral and nude shades have worked for you?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c7zeuv/people_who_find_ilnp_overcoat_flattering_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1c7yxlj</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>LynB - Flaming Zombie</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7yxlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1c7y25x</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Recommendations: a gooood press on nail I can use my own polish on</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c7y25x/recommendations_a_gooood_press_on_nail_i_can_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1c7xvjm</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Feeling Fabulous 🌈</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvn965zx1gvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1c7x9jb</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Scottish Thistle 🪻</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8101m0vwfvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1c7wbeq</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>🏅💚Favorite Chartreuse💚🏅</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7wbeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1c7vpt1</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Does this polish suit my skin tone? Looking for an everyday nude as I work on kicking my nail biting</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7vpt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1c7twtk</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Unexpected Layering Happiness</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7twtk</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1c7rz4u</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Polka dots for Spring! 🫧</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jd4phx6sfevc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1c71m9b</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Whats going on with my nails??</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53s681w9a8vc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1c8k5kr</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Tried sculpting clay for the first time ^-^</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ux0hufbz7lvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1c8jwgd</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Silver chome nails</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j3hwe2u4lvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1c8iuyb</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Undecided about which style to for for this week, so I created some test ones to stare at while I make up my mind 😂</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iye0jc7uskvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1c8efq8</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c12anu0wkjvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1c8dtms</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>I did my nails for America's Beauty show!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8dtms</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1c8cv5s</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Coffee Nails</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nkn7vbm6jvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1c8b59d</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Wht do y’all think? Should I make the base color more nude? (Made by myself)</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8b59d</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1c86ou8</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Floral blue set</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c86ou8</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1c86njp</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Set I just did for the Spring. What y’all think? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucr4z2fhuhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1c85d1w</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Bees🐝🍯</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nr2xa88tkhvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1c84ak7</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Awww 🥰 my new work </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egtd6g5zchvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1c821co</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Hand sculpted Lisa Frank 3D Nail Art Charms🩵🌸🐬 so obsessed with how they came out!!!🩷</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c821co</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1c81vll</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Delicated with a touch of color 🫶🏾</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unfixwccvgvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1c7wjhc</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Check out my rendition of the Van Gogh Exploding Tardis artwork from Doctor Who: The Pandorica Opens. IG@charli.bell.9</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7wjhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1c7we58</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jade extentions for my momma </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uokr00tzpfvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1c7vo2v</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13h1qs0qjfvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1c7uf4q</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>First Post 💗</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6iotl3208fvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1c7tcgh</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Spring airbrush nails</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7tcgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1c7riud</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>first set ever on self</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c7riud</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr 21 08:07:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_21.xlsx
+++ b/data/2024_04_21.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C980"/>
+  <dimension ref="A1:C1129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17093,6 +17093,2539 @@
         </is>
       </c>
     </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1c9c6wv</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>My newest favorite set</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9c6wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1c9c156</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>22F, I’ve been practicing - how am I doing??</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9c156</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1c9aej0</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did the myself! </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x7svexksrvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1c9ad3y</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Lavender cat eye chrome</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9ad3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1c97d2y</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Had one of my classmates paint my natural nails! Credit to @nails.by.caty.2024 on FB</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c97d2y</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1c976we</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Does gel extensions cause same damage as gel polish?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c976we/does_gel_extensions_cause_same_damage_as_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1c95e00</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Most natural looking nails</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c95e00/most_natural_looking_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1c945hm</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Smoky Quartz 😎🚬</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3onv20d2qvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1c937y0</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>How do I find a good nail tech?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c937y0/how_do_i_find_a_good_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1c98upx</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Love my nails!</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2sm8gjmbrvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1c98ozg</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>my 4/20 set!</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c98ozg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1c98kek</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Oil-based nail polish</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c98kek/oilbased_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1c98bhm</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Midnight nails 🖤💙</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c98bhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1c97uel</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Not bad for 2 weeks old 🤭</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vcwjuh41rvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1c97pgq</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>looking for a nail lamp</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c97pgq/looking_for_a_nail_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1c97ljh</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love it </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tl5g1z8lyqvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1c97a0n</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Blue Raspberry &amp; Great Grape</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c97a0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1c9748u</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>🍓Trying press on nails from Shein. What do you think?</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9748u</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1c96qt8</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>🩸🧛</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c96qt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1c96fw5</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do u think of this set? I really love it </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbowbgd6nqvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1c968t7</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>i asked her to make my nails look like olives with pimento. needless to say she understood the assignment.</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wizo5ocdlqvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1c95edf</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Feeling fab!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5eeoz6edqvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1c95cma</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! What can I do? </t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8h1ytv0ycqvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1c95akb</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Alternatives for nail glue</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c95akb/alternatives_for_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1c94uop</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>New Set🧜‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c94uop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1c94uhs</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>JJK Sukuna Nails</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c94uhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1c94q4p</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Finally grew out my natural nails</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c94q4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1c94gpm</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Current nails ☺️🌸</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c94gpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1c944nq</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Floral Nails</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c944nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1c92w2m</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>First time making gel press ons!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c92w2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1c92u8g</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Bunny nails(done by me)</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c92u8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1c92cb2</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>I got a fresh set today and I’m SO in love with the design</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c92cb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1c92aqh</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>I’m in love💅🏻💖🖤</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1mwly8wmpvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1c929ab</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Fresh set L then R</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c929ab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1c91uzr</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails not drying properly </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c91uzr/nails_not_drying_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1c8xtpn</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Air bubbles ;-( </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8xtpn/air_bubbles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1c91a21</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Sticking with press-ons for a while</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c91a21</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1c919n6</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>fresh gel manicure. 🩷</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jltl7jpepvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1c913yw</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Diy- acrylic extension to my broken brittle nails(winter was harsh😬😅) finished with gel polish and matte top coat…not perfect, but definitely wallet friendly 🤭🤭 (habitual lurker, first time poster)</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c913yw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1c90ni7</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Haven’t had my nails done in what felt for sooo long🩷</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c90ni7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1c90jsj</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Birthday present for my mom</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c90jsj/birthday_present_for_my_mom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1c90gn0</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Having a shitty day and then this happened at work actually almost cried. Anyone try the teabag? Method? </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki2n2u0f8pvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1c8zl6s</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>First set in over 2 years</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8zl6s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1c8z82p</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Left hand done</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j0zdb5nryovc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1c8z34t</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>How much do you tip at a nail salon?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8z34t/how_much_do_you_tip_at_a_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1c8y4rn</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Fresh Talons</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ksehp4o8qovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1c8upfj</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Can someone help me put together a design or moodboard for ethereal / Iris Van Herpen inspired nails? I don't speak the main language of where I'm living now (Netherlands). I'm worried I wouldn't explain well and similar metal and dripping metal isn't what I'd want on all nails.</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8upfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1c8vl27</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>In the name of the moon, I’ll punish you!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8vl27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1c8vwn7</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Test Nail - Inspiration: Opal ✨</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4suyi0jl9ovc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1c8ximy</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>please help</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8ximy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1c8wypy</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Strayed away from pastels this week</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8wypy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1c8ws2a</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Is my cuticle oil removing my gel manicure?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8ws2a/is_my_cuticle_oil_removing_my_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1c8wk8g</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Several few months ago my builder gels leaked from the pot and into my nail bag and ziploc bag and I can't clean it well. It's now separated or changed appearance. How can I clean it and get rid of the smell? Also how to keep clean when using from pots?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8wk8g/several_few_months_ago_my_builder_gels_leaked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1c8w4zc</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>New nails ✨</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8w4zc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1c8w1r3</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>I don’t know what’s missing?Like I don’t quite like this set.Should I just replace the heart shaped gem? Make it like the middle finger instead?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8w1r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1c8vy37</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>short nails❤️</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de9y5sqw9ovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1c8v2y9</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>I had them done yesterday and love them 💙</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8v2y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1c8uypt</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Is is weird or unprofessional to ask a tech to pre make a set of nails to put on in a later appointment? I am just looking at some more complicated designs, if a nail tech would find this weird. Have you had any experiences with this?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8uypt/is_is_weird_or_unprofessional_to_ask_a_tech_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1c8us5z</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Frenchies in brown and dot detail, I love</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ackwibyx0ovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1c8u5vs</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Many colors</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krbwefj2wnvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1c8u2e2</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89ofqxwbvnvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1c8u0bf</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Is it possible my nails are too short for polygel? They keep coming off no matter what I try. Professional acrylic is absolutely fine. I basically have no white edge due to biting and strong cleaning soap at work.</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8u0bf/is_it_possible_my_nails_are_too_short_for_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1c8u09w</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Rainbow with a twist ❤️ 🌈</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8u09w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1c8txeb</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Lost my 120w Sun nail lamp's cable. What is that type called? I'm using an EU plug.</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8txeb/lost_my_120w_sun_nail_lamps_cable_what_is_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1c8tdzi</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Did a new set, I'm so proud of it!!!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8tdzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1c8tdxm</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸🎀💕</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8tdxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1c8slfe</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Basic but I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rq65khnxjnvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1c8sbzy</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>When your nail lady hooks you up with pretty nails 😍💅🏼</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1d519nxhnvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1c8s40q</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I go back? </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d66eqa8gnvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1c8oat5</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>I want to learn how to shape my nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8oat5/i_want_to_learn_how_to_shape_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1c8i9jm</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>First time working with loose glitter!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sbfe299mkvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1c8qvmc</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>What is this new nail art method ? Help !</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8qvmc/what_is_this_new_nail_art_method_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1c8rf1i</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Do stubbies get love too?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/off0zdmoanvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1c8qz0m</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Might be my fav set😍</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc9lifg67nvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1c8pwu1</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>what nail shape do you think would best suit my hands/fingers??</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8pwu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1c8ookn</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Blue one</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmsxt6aenmvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1c8o4cw</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Loving this sage green 🌿</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2gbb5qzyhmvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1c8nvih</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8nvih/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1c8nq1d</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Nails I did a few weeks ago 💕</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8nq1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1c8nja5</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Using non-hybrid gel color</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c8nja5/using_nonhybrid_gel_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1c8ku01</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Handmade Custom Set by me 💗</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9e6wnl5glvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1c8dgpq</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>matte black nails</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8dgpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1c9c4tx</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Did my boyfriends mom's nails.</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9c4tx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1c9b4in</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Robin-egg thermal polish</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9b4in</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1c9b13u</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Do NailzKatKat rubber base coats and gel polishes contain HEMA?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c9b13u/do_nailzkatkat_rubber_base_coats_and_gel_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1c994m6</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Found my new obsession</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c994m6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1c9926f</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Man thank yall for your growth tips!</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9926f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1c98tm3</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Dupe for Holo Taco Aquafoil ??</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh0cv72bbrvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1c98qk2</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>my 4/20 nails!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c98qk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1c98hkq</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Mooncat "Maelstrom"</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6fm2swt7rvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1c98hds</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Can you combine topcoats of different brands?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b535rsno7rvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1c97tgm</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>ILNP Juliette ✨</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1ccieo0r0rvc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1c95son</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>I finally found my perfect nude 😎</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzssa061hqvc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1c96tin</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Does any one know of a polish similar to this shade? Thanks :)</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c96tin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1c96c4h</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Ugh throw me in the trash. Finally picked up more swatch sticks and labeled them the wrong way</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueg71ug9mqvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1c9658f</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Beaux Reves Blooming Azalea (PPU Jan ‘24) 🌺✨</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9658f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1c95mjb</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Can someone help me recreate this dye-stained polish?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c95mjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1c95ii9</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>But Do Aliens Believe in Me? ~ DVN</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c95ii9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1c95g8t</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>New to polish; are all holos also kind of shimmers?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c95g8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1c951vh</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>When in doubt, add Moondust.</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r17cpar6aqvc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1c94ihp</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>I just painted these and honestly I LOVE how they came out !</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c94ihp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1c94gk3</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Added little flowers. Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c94gk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1c93psb</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>I gasped when I saw this bottle for the first time... But I kind of hate it on my nails.</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c93psb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1c932xo</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Just Another First-time Builder Gel Post</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c932xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1c92efj</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Choose Life for 4/20 🍃</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c92efj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1c91fjs</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>🌜🌚🌗</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c91fjs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1c91cab</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Pre-birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn0lc3oafpvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1c915qa</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Spring pop🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77yv2bgvdpvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1c90pic</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First try at a gradient! </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqm984ubapvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1c90ff5</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>J. Hannah Polish 50% with "liltreat" coupon code</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c90ff5/j_hannah_polish_50_with_liltreat_coupon_code/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1c8zlx7</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>🌸 Cherry blossom season 🌸</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8zlx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1c8x2pw</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>This one’s for the lesbians</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8x2pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1c8z1zz</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Yucca in Bloom</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8z1zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1c8y5ei</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Flower power 🌸</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8y5ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1c8x7rh</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>AEngland Michael</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9qe162gjovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1c8wzql</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>💚🌲🌴🐸🦖🍏🪀🪲♻️</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8wzql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1c8wel9</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Just got my Mooncat order for the new collection, this is Siren’s Revenge next to Full Scream Ahead (and every other light green I have) for those wondering how similar they are</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8wel9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1c8w3jh</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>DVN dotticure</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayhjwyx3bovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1c8v6az</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Is Cirque Colors not doing a 420 collection this year?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8v6az/is_cirque_colors_not_doing_a_420_collection_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1c8uxuh</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Strawberry Macaron</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8esings32ovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1c8usdi</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Happy 420🌲</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8usdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1c8uoqd</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>ILNP - Deep Space (Unmagnetized) 😍</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4fgc2170ovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1c8td9n</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Dragon scales for 420</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8td9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1c8t8pt</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Earth Day Nails</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8t8pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1c8sbsc</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>I love these kinds of blues 💙</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zr151ssvhnvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1c8rwv7</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>I'm genuinely impressed how well this is holding up</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8rwv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1c8rvbp</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Photochromatic help?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8rvbp/photochromatic_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1c8r1rl</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Dusky pink feat gold shimmer</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8r1rl/dusky_pink_feat_gold_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1c8qiia</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Base coat/top coat - do I really need both?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8qiia/base_coattop_coat_do_i_really_need_both/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1c8q78n</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Oh how I love holo🌈</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8q78n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1c8pp5y</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>BKL — Nessian offering emotional support for my graduation!!!!!!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8pp5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1c8phrw</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>So happy with how cute this turned out!</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad9nnqauumvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1c8pfm4</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Proximal nail folds were really hard to push back. How can I improve?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c8pfm4/proximal_nail_folds_were_really_hard_to_push_back/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1c8on3h</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>🏅💚Favorite Emerald💚🏅</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8on3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1c8nk1t</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>LA Colors - Culture, glossy and matte</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8nk1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1c8n5pt</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>At least it's just the tip</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8n5pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1c8lxyz</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Inspiration Vs what I got</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8lxyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1c8lggx</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Flowers with alternating colors :)</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8lggx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1c8kpzj</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Layering for perfection</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8kpzj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1c9a9rm</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>New set! Any tips please!!</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c9a9rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1c996zw</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Rose Quartz Inspired Custom Press Ons</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e5h59ascfrvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1c987zx</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried bee nails </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sks972j15rvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1c97szd</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went with a marble design </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vmjbgpp0rvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1c8zt73</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Black + White Tropical Nails 🌿🖤🌴🤍</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8zt73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1c8z69p</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love this desing i made for me , do you? </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytetb8idyovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1c8xdfq</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>What do you think about my new work? 🐚🌊</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpc7cs9mkovc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1c8u09a</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>🌜🌚🌗</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8u09a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1c8rwp1</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>More Spring Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mn1dvf9oenvc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1c8lzze</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Some marble practice</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c8lzze</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>